<commit_message>
added python file for excel calc
</commit_message>
<xml_diff>
--- a/toy gravity model.xlsx
+++ b/toy gravity model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ltavasszy\Documents\My Documents\onderwijs\ct4840\2024 CIEM6210 CIEQ6213 SEN173A\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evert\Documents\TU-Delft\TIL Master\CIEQ6213 Freight Transport Networks and Systems\CIEQ6213_Freight_Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60447CDC-BF17-4B81-BF5B-250029465BF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB0DE693-2987-4134-AB6E-67E93EA927A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="gravity" sheetId="1" r:id="rId1"/>
@@ -283,7 +283,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -301,7 +301,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -808,7 +808,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1230,7 +1230,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3633,20 +3633,20 @@
   <dimension ref="A1:AC39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="14" max="14" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:29" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="24" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:29" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="25" t="s">
         <v>0</v>
       </c>
@@ -3660,11 +3660,11 @@
         <v>-0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="20"/>
       <c r="Q6" s="20"/>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="C7" s="1" t="s">
         <v>1</v>
       </c>
@@ -3712,7 +3712,7 @@
       <c r="AB7" s="4"/>
       <c r="AC7" s="4"/>
     </row>
-    <row r="8" spans="1:29" ht="21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:29" ht="21" x14ac:dyDescent="0.4">
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
@@ -3769,7 +3769,7 @@
       <c r="AB8" s="4"/>
       <c r="AC8" s="4"/>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>2</v>
       </c>
@@ -3825,7 +3825,7 @@
       <c r="AB9" s="4"/>
       <c r="AC9" s="4"/>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
@@ -3881,7 +3881,7 @@
       <c r="AB10" s="4"/>
       <c r="AC10" s="4"/>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -3937,7 +3937,7 @@
       <c r="AB11" s="4"/>
       <c r="AC11" s="4"/>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
@@ -3993,7 +3993,7 @@
       <c r="AB12" s="4"/>
       <c r="AC12" s="4"/>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>6</v>
       </c>
@@ -4049,7 +4049,7 @@
       <c r="AB13" s="4"/>
       <c r="AC13" s="4"/>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>7</v>
       </c>
@@ -4105,7 +4105,7 @@
       <c r="AB14" s="4"/>
       <c r="AC14" s="4"/>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
         <v>8</v>
       </c>
@@ -4161,7 +4161,7 @@
       <c r="AB15" s="4"/>
       <c r="AC15" s="4"/>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>9</v>
       </c>
@@ -4217,7 +4217,7 @@
       <c r="AB16" s="4"/>
       <c r="AC16" s="4"/>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>10</v>
       </c>
@@ -4273,7 +4273,7 @@
       <c r="AB17" s="4"/>
       <c r="AC17" s="4"/>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
         <v>11</v>
       </c>
@@ -4330,7 +4330,7 @@
       <c r="AB18" s="4"/>
       <c r="AC18" s="4"/>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
       <c r="Q19" s="3">
         <v>200</v>
       </c>
@@ -4350,7 +4350,7 @@
       <c r="AB19" s="4"/>
       <c r="AC19" s="4"/>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="Q20" s="3">
         <v>220</v>
       </c>
@@ -4370,7 +4370,7 @@
       <c r="AB20" s="4"/>
       <c r="AC20" s="4"/>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
       <c r="Q21" s="3">
         <v>240</v>
       </c>
@@ -4390,7 +4390,7 @@
       <c r="AB21" s="4"/>
       <c r="AC21" s="4"/>
     </row>
-    <row r="22" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:29" ht="18" x14ac:dyDescent="0.35">
       <c r="A22" s="25" t="s">
         <v>14</v>
       </c>
@@ -4413,7 +4413,7 @@
       <c r="AB22" s="4"/>
       <c r="AC22" s="4"/>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
       <c r="Q23" s="3">
         <v>280</v>
       </c>
@@ -4433,7 +4433,7 @@
       <c r="AB23" s="4"/>
       <c r="AC23" s="4"/>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B24" s="7" t="s">
         <v>15</v>
       </c>
@@ -4489,7 +4489,7 @@
       <c r="AB24" s="4"/>
       <c r="AC24" s="4"/>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
         <v>16</v>
       </c>
@@ -4548,7 +4548,7 @@
       <c r="AB25" s="4"/>
       <c r="AC25" s="4"/>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A26" s="9"/>
       <c r="N26" s="14"/>
       <c r="Q26" s="3">
@@ -4570,7 +4570,7 @@
       <c r="AB26" s="4"/>
       <c r="AC26" s="4"/>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A27" s="11">
         <v>124</v>
       </c>
@@ -4644,7 +4644,7 @@
       <c r="AB27" s="4"/>
       <c r="AC27" s="4"/>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A28" s="11">
         <v>26</v>
       </c>
@@ -4718,7 +4718,7 @@
       <c r="AB28" s="4"/>
       <c r="AC28" s="4"/>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A29" s="11">
         <v>19</v>
       </c>
@@ -4792,7 +4792,7 @@
       <c r="AB29" s="4"/>
       <c r="AC29" s="4"/>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A30" s="11">
         <v>97</v>
       </c>
@@ -4866,7 +4866,7 @@
       <c r="AB30" s="4"/>
       <c r="AC30" s="4"/>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A31" s="11">
         <v>157</v>
       </c>
@@ -4940,7 +4940,7 @@
       <c r="AB31" s="4"/>
       <c r="AC31" s="4"/>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A32" s="11">
         <v>38</v>
       </c>
@@ -5014,7 +5014,7 @@
       <c r="AB32" s="4"/>
       <c r="AC32" s="4"/>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A33" s="11">
         <v>182</v>
       </c>
@@ -5088,7 +5088,7 @@
       <c r="AB33" s="4"/>
       <c r="AC33" s="4"/>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A34" s="11">
         <v>290</v>
       </c>
@@ -5162,7 +5162,7 @@
       <c r="AB34" s="4"/>
       <c r="AC34" s="4"/>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A35" s="11">
         <v>75</v>
       </c>
@@ -5231,7 +5231,7 @@
       <c r="AB35" s="4"/>
       <c r="AC35" s="4"/>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A36" s="11">
         <v>98</v>
       </c>
@@ -5301,7 +5301,7 @@
       <c r="AB36" s="4"/>
       <c r="AC36" s="4"/>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A37" s="11">
         <v>114</v>
       </c>
@@ -5371,61 +5371,61 @@
       <c r="AB37" s="4"/>
       <c r="AC37" s="4"/>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B38" s="14" t="s">
         <v>26</v>
       </c>
       <c r="C38" s="14">
-        <f>SUM(C27:C37)</f>
+        <f t="shared" ref="C38:N38" si="13">SUM(C27:C37)</f>
         <v>13839.45955317178</v>
       </c>
       <c r="D38" s="14">
-        <f>SUM(D27:D37)</f>
+        <f t="shared" si="13"/>
         <v>5946.6800612859633</v>
       </c>
       <c r="E38" s="14">
-        <f>SUM(E27:E37)</f>
+        <f t="shared" si="13"/>
         <v>5099.8646612267221</v>
       </c>
       <c r="F38" s="14">
-        <f>SUM(F27:F37)</f>
+        <f t="shared" si="13"/>
         <v>24520.585528720676</v>
       </c>
       <c r="G38" s="14">
-        <f>SUM(G27:G37)</f>
+        <f t="shared" si="13"/>
         <v>36928.273623231384</v>
       </c>
       <c r="H38" s="14">
-        <f>SUM(H27:H37)</f>
+        <f t="shared" si="13"/>
         <v>13119.081191590885</v>
       </c>
       <c r="I38" s="14">
-        <f>SUM(I27:I37)</f>
+        <f t="shared" si="13"/>
         <v>52354.615990944018</v>
       </c>
       <c r="J38" s="14">
-        <f>SUM(J27:J37)</f>
+        <f t="shared" si="13"/>
         <v>82728.583026309527</v>
       </c>
       <c r="K38" s="14">
-        <f>SUM(K27:K37)</f>
+        <f t="shared" si="13"/>
         <v>13530.604976070614</v>
       </c>
       <c r="L38" s="14">
-        <f>SUM(L27:L37)</f>
+        <f t="shared" si="13"/>
         <v>30397.084041663984</v>
       </c>
       <c r="M38" s="14">
-        <f>SUM(M27:M37)</f>
+        <f t="shared" si="13"/>
         <v>15201.717169244213</v>
       </c>
       <c r="N38" s="14">
-        <f>SUM(N27:N37)</f>
+        <f t="shared" si="13"/>
         <v>293666.54982345976</v>
       </c>
       <c r="O38" s="2"/>
     </row>
-    <row r="39" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="N39" s="18">
         <v>293667</v>
       </c>
@@ -5444,17 +5444,17 @@
       <selection activeCell="J10" activeCellId="1" sqref="H10:H20 J10:J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E8" s="1" t="s">
         <v>18</v>
       </c>
@@ -5477,10 +5477,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="5:11" x14ac:dyDescent="0.3">
       <c r="H9" s="15"/>
     </row>
-    <row r="10" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E10" s="1" t="s">
         <v>1</v>
       </c>
@@ -5501,7 +5501,7 @@
         <v>13839.45955317178</v>
       </c>
     </row>
-    <row r="11" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E11" s="1" t="s">
         <v>2</v>
       </c>
@@ -5522,7 +5522,7 @@
         <v>5946.6800612859633</v>
       </c>
     </row>
-    <row r="12" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E12" s="1" t="s">
         <v>3</v>
       </c>
@@ -5543,7 +5543,7 @@
         <v>5099.8646612267221</v>
       </c>
     </row>
-    <row r="13" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E13" s="1" t="s">
         <v>4</v>
       </c>
@@ -5564,7 +5564,7 @@
         <v>24520.585528720676</v>
       </c>
     </row>
-    <row r="14" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E14" s="1" t="s">
         <v>5</v>
       </c>
@@ -5585,7 +5585,7 @@
         <v>36928.273623231384</v>
       </c>
     </row>
-    <row r="15" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E15" s="1" t="s">
         <v>6</v>
       </c>
@@ -5606,7 +5606,7 @@
         <v>13119.081191590885</v>
       </c>
     </row>
-    <row r="16" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E16" s="1" t="s">
         <v>7</v>
       </c>
@@ -5627,7 +5627,7 @@
         <v>52354.615990944018</v>
       </c>
     </row>
-    <row r="17" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E17" s="1" t="s">
         <v>8</v>
       </c>
@@ -5648,7 +5648,7 @@
         <v>82728.583026309527</v>
       </c>
     </row>
-    <row r="18" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E18" s="1" t="s">
         <v>9</v>
       </c>
@@ -5669,7 +5669,7 @@
         <v>13530.604976070614</v>
       </c>
     </row>
-    <row r="19" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E19" s="1" t="s">
         <v>10</v>
       </c>
@@ -5690,7 +5690,7 @@
         <v>30397.084041663984</v>
       </c>
     </row>
-    <row r="20" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E20" s="1" t="s">
         <v>11</v>
       </c>
@@ -5711,7 +5711,7 @@
         <v>15201.717169244213</v>
       </c>
     </row>
-    <row r="21" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E21" s="1"/>
     </row>
   </sheetData>

</xml_diff>